<commit_message>
gamma prior on root respiration
</commit_message>
<xml_diff>
--- a/Cogongrass_trait_sampling/root_respiration_2019/Cogongrass_Respiration_Biomass_2019.xlsx
+++ b/Cogongrass_trait_sampling/root_respiration_2019/Cogongrass_Respiration_Biomass_2019.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tess/Documents/work/SERDP_Project/Cogongrass_trait_sampling/root_respiration_2019/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7F8C2C04-B8E4-BB44-BFA2-482F3C24E4CB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{280424E7-3C9D-4F4E-9CDC-46919C1DA051}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="12">
   <si>
     <t>Number</t>
   </si>
@@ -47,6 +47,15 @@
   </si>
   <si>
     <t>Rhyzomes were measured during an issue with IRGA</t>
+  </si>
+  <si>
+    <t>combo dry g</t>
+  </si>
+  <si>
+    <t>Combo dry g colum is made up of the sum of the dry g of corresponding number columns</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
@@ -404,13 +413,15 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -427,10 +438,13 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -446,8 +460,15 @@
       <c r="E2" s="1">
         <v>4.04</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F2">
+        <f>SUM(B2, E2)</f>
+        <v>4.4442000000000004</v>
+      </c>
+      <c r="G2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -463,8 +484,12 @@
       <c r="E3" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F3">
+        <f t="shared" ref="F3:F22" si="0">SUM(B3, E3)</f>
+        <v>4.508</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -480,8 +505,12 @@
       <c r="E4" s="1">
         <v>4.32</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F4">
+        <f t="shared" si="0"/>
+        <v>4.9024000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -497,8 +526,12 @@
       <c r="E5" s="1">
         <v>4.97</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>5.6918999999999995</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -514,8 +547,12 @@
       <c r="E6" s="1">
         <v>5.14</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>6.1084999999999994</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -531,8 +568,12 @@
       <c r="E7" s="1">
         <v>3.97</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>4.8380999999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -548,11 +589,14 @@
       <c r="E8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -568,8 +612,12 @@
       <c r="E9" s="1">
         <v>5.07</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>6.1203000000000003</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -585,8 +633,12 @@
       <c r="E10" s="1">
         <v>5.1100000000000003</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>6.016</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -602,8 +654,12 @@
       <c r="E11" s="1">
         <v>5.6</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F11">
+        <f t="shared" si="0"/>
+        <v>6.7374999999999998</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -619,8 +675,11 @@
       <c r="E12" s="1">
         <v>6.32</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -636,8 +695,11 @@
       <c r="E13" s="1">
         <v>6.3</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -653,11 +715,14 @@
       <c r="E14" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="F14" t="s">
+        <v>11</v>
+      </c>
+      <c r="G14" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -673,8 +738,11 @@
       <c r="E15" s="1">
         <v>6.35</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -690,8 +758,11 @@
       <c r="E16" s="1">
         <v>8</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -707,8 +778,11 @@
       <c r="E17" s="1">
         <v>6.81</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F17" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -724,8 +798,11 @@
       <c r="E18" s="1">
         <v>7.55</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F18" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -741,8 +818,11 @@
       <c r="E19" s="1">
         <v>7.84</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F19" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -758,8 +838,11 @@
       <c r="E20" s="1">
         <v>7.17</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F20" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -775,8 +858,11 @@
       <c r="E21" s="1">
         <v>7.43</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F21" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -791,6 +877,9 @@
       </c>
       <c r="E22" s="1">
         <v>5.57</v>
+      </c>
+      <c r="F22" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>